<commit_message>
Added crds_plan.txt to docs, list of activities for next few months Recolored a requirement in metrics
git-svn-id: https://aeon.stsci.edu/ssb/svn/crds/trunk@893 0d8f46c8-9b30-49d0-b470-0f6283dc92e8
</commit_message>
<xml_diff>
--- a/docs/HST_Upgrade_Reqs_Metrics_03-18-13-edit.xlsx
+++ b/docs/HST_Upgrade_Reqs_Metrics_03-18-13-edit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1400" windowWidth="31120" windowHeight="25080" tabRatio="890" activeTab="1"/>
+    <workbookView xWindow="9200" yWindow="1320" windowWidth="31120" windowHeight="25080" tabRatio="890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CRDS_Reqs" sheetId="5" r:id="rId1"/>
@@ -1473,8 +1473,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2172,7 +2190,7 @@
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="153">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2246,6 +2264,9 @@
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2319,6 +2340,9 @@
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2747,11 +2771,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140543736"/>
-        <c:axId val="2140546888"/>
+        <c:axId val="-2132875048"/>
+        <c:axId val="-2132871832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140543736"/>
+        <c:axId val="-2132875048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140546888"/>
+        <c:crossAx val="-2132871832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2787,7 +2811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140546888"/>
+        <c:axId val="-2132871832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,7 +2880,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140543736"/>
+        <c:crossAx val="-2132875048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -3226,11 +3250,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140636456"/>
-        <c:axId val="2140639640"/>
+        <c:axId val="-2133445368"/>
+        <c:axId val="-2133448488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140636456"/>
+        <c:axId val="-2133445368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3258,7 +3282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140639640"/>
+        <c:crossAx val="-2133448488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3266,7 +3290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140639640"/>
+        <c:axId val="-2133448488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3326,7 +3350,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140636456"/>
+        <c:crossAx val="-2133445368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3687,11 +3711,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140687912"/>
-        <c:axId val="2140691096"/>
+        <c:axId val="-2133496696"/>
+        <c:axId val="-2133499896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140687912"/>
+        <c:axId val="-2133496696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3719,7 +3743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140691096"/>
+        <c:crossAx val="-2133499896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3727,7 +3751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140691096"/>
+        <c:axId val="-2133499896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3787,7 +3811,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140687912"/>
+        <c:crossAx val="-2133496696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -4176,11 +4200,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140741512"/>
-        <c:axId val="2140744696"/>
+        <c:axId val="-2133550296"/>
+        <c:axId val="-2133553496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140741512"/>
+        <c:axId val="-2133550296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4208,7 +4232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140744696"/>
+        <c:crossAx val="-2133553496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4216,7 +4240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140744696"/>
+        <c:axId val="-2133553496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4277,7 +4301,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2140741512"/>
+        <c:crossAx val="-2133550296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -4518,11 +4542,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2140795576"/>
-        <c:axId val="2140798856"/>
+        <c:axId val="-2133604360"/>
+        <c:axId val="-2133607656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140795576"/>
+        <c:axId val="-2133604360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4557,7 +4581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140798856"/>
+        <c:crossAx val="-2133607656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4565,7 +4589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140798856"/>
+        <c:axId val="-2133607656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4641,7 +4665,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140795576"/>
+        <c:crossAx val="-2133604360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5203,8 +5227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6698,7 +6722,7 @@
   <dimension ref="A1:AA170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" outlineLevelCol="7" x14ac:dyDescent="0"/>
@@ -8015,20 +8039,12 @@
       <c r="M32" s="79">
         <v>3</v>
       </c>
-      <c r="N32" s="69">
-        <v>2</v>
-      </c>
+      <c r="N32" s="80"/>
       <c r="O32" s="89"/>
-      <c r="P32" s="69">
-        <v>2</v>
-      </c>
-      <c r="Q32" s="69">
-        <v>2</v>
-      </c>
+      <c r="P32" s="80"/>
+      <c r="Q32" s="80"/>
       <c r="R32" s="89"/>
-      <c r="S32" s="79">
-        <v>3</v>
-      </c>
+      <c r="S32" s="80"/>
       <c r="T32" s="80"/>
     </row>
     <row r="33" spans="1:23">
@@ -8285,21 +8301,21 @@
       </c>
       <c r="N39" s="76">
         <f>SUM(N2:N37)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O39" s="64"/>
       <c r="P39" s="76">
         <f>SUM(P2:P37)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q39" s="76">
         <f>SUM(Q2:Q37)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R39" s="64"/>
       <c r="S39" s="76">
         <f>SUM(S2:S37)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="T39" s="76">
         <f>SUM(T2:T37)</f>
@@ -11431,21 +11447,21 @@
       </c>
       <c r="N153" s="76">
         <f>SUM(N39,N76,N91,N103,N110,N115,N125,N135,N145)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O153" s="64"/>
       <c r="P153" s="76">
         <f>SUM(P39,P76,P91,P103,P110,P115,P125,P135,P145)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q153" s="76">
         <f>SUM(Q39,Q76,Q91,Q103,Q110,Q115,Q125,Q135,Q145)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R153" s="64"/>
       <c r="S153" s="76">
         <f>SUM(S39,S76,S91,S103,S110,S115,S125,S135,S145)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="T153" s="76">
         <f>SUM(T39,T76,T91,T103,T110,T115,T125,T135,T145)</f>
@@ -11546,21 +11562,21 @@
       </c>
       <c r="N157" s="76">
         <f>SUM(N39)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O157" s="64"/>
       <c r="P157" s="76">
         <f>SUM(P39)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q157" s="76">
         <f>SUM(Q39)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R157" s="64"/>
       <c r="S157" s="76">
         <f>SUM(S39)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="T157" s="76">
         <f>SUM(T39)</f>

</xml_diff>